<commit_message>
Major updates to toolbox
</commit_message>
<xml_diff>
--- a/mnt/city-directories/02-process-output/fu_osmpt.xlsx
+++ b/mnt/city-directories/02-process-output/fu_osmpt.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>health</t>
+          <t>police</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,14 +474,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>police</t>
+          <t>schools</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Everything compiled in text options
</commit_message>
<xml_diff>
--- a/mnt/city-directories/02-process-output/fu_osmpt.xlsx
+++ b/mnt/city-directories/02-process-output/fu_osmpt.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>police</t>
+          <t>health</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,16 +474,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>schools</t>
+          <t>police</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>schools</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change to elev and age labels
</commit_message>
<xml_diff>
--- a/mnt/city-directories/02-process-output/fu_osmpt.xlsx
+++ b/mnt/city-directories/02-process-output/fu_osmpt.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>4.166666666666666</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to all graphs
</commit_message>
<xml_diff>
--- a/mnt/city-directories/02-process-output/fu_osmpt.xlsx
+++ b/mnt/city-directories/02-process-output/fu_osmpt.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>7.692307692307693</v>
       </c>
     </row>
     <row r="3">
@@ -478,29 +478,45 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>fire</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>schools</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>66.66666666666666</v>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>138</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.173913043478261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>